<commit_message>
agregado de actualizaciones en los listados y fotos de recuperatorios
</commit_message>
<xml_diff>
--- a/inasistencias-4b-elecYsiscom-tp/alumnos-4b-ElecYsisCom-tp.xlsx
+++ b/inasistencias-4b-elecYsiscom-tp/alumnos-4b-ElecYsisCom-tp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="133">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -516,7 +516,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,35 +529,44 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <b val="1"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="12"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <color rgb="FF006600"/>
+        <sz val="12"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF232629"/>
-          <bgColor rgb="FFFFFFFF"/>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <color rgb="FFCC0000"/>
+        <sz val="12"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -586,7 +595,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -643,13 +652,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.63671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
@@ -1474,6 +1483,9 @@
       <c r="U16" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T16,R16,P16,N16,L16),0)</f>
         <v>3</v>
+      </c>
+      <c r="V16" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,13 +1584,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W12" activeCellId="0" sqref="W12"/>
+      <selection pane="topLeft" activeCell="V17" activeCellId="0" sqref="V17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.57"/>
@@ -1725,7 +1737,7 @@
       <c r="T2" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T2,R2,P2,N2,L2),0)</f>
         <v>8</v>
       </c>
@@ -1788,7 +1800,7 @@
       <c r="T3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T3,R3,P3,N3,L3),0)</f>
         <v>9</v>
       </c>
@@ -1854,7 +1866,7 @@
       <c r="T4" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T4,R4,P4,N4,L4),0)</f>
         <v>6</v>
       </c>
@@ -1914,7 +1926,7 @@
       <c r="T5" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="U5" s="0" t="n">
+      <c r="U5" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T5,R5,P5,N5,L5),0)</f>
         <v>7</v>
       </c>
@@ -1974,7 +1986,7 @@
       <c r="T6" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U6" s="0" t="n">
+      <c r="U6" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T6,R6,P6,N6,L6),0)</f>
         <v>7</v>
       </c>
@@ -2037,7 +2049,7 @@
       <c r="T7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U7" s="0" t="n">
+      <c r="U7" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T7,R7,P7,N7,L7),0)</f>
         <v>8</v>
       </c>
@@ -2103,7 +2115,7 @@
       <c r="T8" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U8" s="0" t="n">
+      <c r="U8" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T8,R8,P8,N8,L8),0)</f>
         <v>7</v>
       </c>
@@ -2169,7 +2181,7 @@
       <c r="T9" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U9" s="0" t="n">
+      <c r="U9" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T9,R9,P9,N9,L9),0)</f>
         <v>8</v>
       </c>
@@ -2226,7 +2238,7 @@
       <c r="T10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U10" s="0" t="n">
+      <c r="U10" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T10,R10,P10,N10,L10),0)</f>
         <v>8</v>
       </c>
@@ -2292,7 +2304,7 @@
       <c r="T11" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U11" s="0" t="n">
+      <c r="U11" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T11,R11,P11,N11,L11),0)</f>
         <v>7</v>
       </c>
@@ -2349,7 +2361,7 @@
       <c r="T12" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="U12" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T12,R12,P12,N12,L12),0)</f>
         <v>9</v>
       </c>
@@ -2409,7 +2421,7 @@
       <c r="T13" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="U13" s="0" t="n">
+      <c r="U13" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T13,R13,P13,N13,L13),0)</f>
         <v>6</v>
       </c>
@@ -2466,7 +2478,7 @@
       <c r="T14" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="U14" s="0" t="n">
+      <c r="U14" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T14,R14,P14,N14,L14),0)</f>
         <v>7</v>
       </c>
@@ -2526,7 +2538,7 @@
       <c r="T15" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="U15" s="0" t="n">
+      <c r="U15" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T15,R15,P15,N15,L15),0)</f>
         <v>7</v>
       </c>
@@ -2586,9 +2598,12 @@
       <c r="T16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U16" s="0" t="n">
+      <c r="U16" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T16,R16,P16,N16,L16),0)</f>
         <v>4</v>
+      </c>
+      <c r="V16" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2643,20 +2658,32 @@
       <c r="T17" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="U17" s="0" t="n">
+      <c r="U17" s="4" t="n">
         <f aca="false">ROUND(AVERAGE(T17,R17,P17,N17,L17),0)</f>
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J17">
-    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K17">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"TEP"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:U17">
+    <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="notBetween" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>4</formula>
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2680,7 +2707,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.95"/>
@@ -3126,7 +3153,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.57"/>
   </cols>

</xml_diff>

<commit_message>
actualizacion de asistencias al 14 de oct
</commit_message>
<xml_diff>
--- a/inasistencias-4b-elecYsiscom-tp/alumnos-4b-ElecYsisCom-tp.xlsx
+++ b/inasistencias-4b-elecYsiscom-tp/alumnos-4b-ElecYsisCom-tp.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="154">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -49,9 +49,120 @@
     <t xml:space="preserve">competencia</t>
   </si>
   <si>
+    <t xml:space="preserve">nogz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nota</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ivan</t>
   </si>
   <si>
+    <t xml:space="preserve">ALTAMIRANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matias2511.altamirano@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Hidroelectrica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">olimpiadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiplicador de rmp, ladron de joules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">me gsta, caja de madera para la proxima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar modelos de aspas, hacer pruebas con 2 tipos de motores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impresion de las helices, se mejoro el modelo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivan Benjamín</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CABALLERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49898249@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matías Andrés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CETERA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50276187@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asai Nitzana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trinidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matruia81@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hay que evaluar el tama del eje y la velocidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ulises Nicolas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIMÉNEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50156642@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-Pancho pila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hacer ladron de jouls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hacer un modelo con 3 pancho pilas, modelos de linternas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiago Benjamín</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELLO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49676837@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ladron de joules, conseguir leds, modelos de linternas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nazarena Valentina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEVEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47869497@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rafael Bautista</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACUÑA</t>
   </si>
   <si>
@@ -61,19 +172,16 @@
     <t xml:space="preserve">3-solar</t>
   </si>
   <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
     <t xml:space="preserve">reparar, arduino, sensor de humedad, sensor de luz</t>
   </si>
   <si>
     <t xml:space="preserve">sanata</t>
   </si>
   <si>
-    <t xml:space="preserve">Ivan Benjamín</t>
+    <t xml:space="preserve">me gusta el modelo encontrado, el piso de la maqueta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Nahuel</t>
   </si>
   <si>
     <t xml:space="preserve">AGUERRE</t>
@@ -82,49 +190,10 @@
     <t xml:space="preserve">49627703@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Matías Andrés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALTAMIRANO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matias2511.altamirano@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-Hidroelectrica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">olimpiadas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multiplicador de rmp, ladron de joules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">me gsta, caja de madera para la proxima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asai Nitzana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CABALLERO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49898249@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ulises Nicolas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CETERA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50276187@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thiago Benjamín</t>
+    <t xml:space="preserve">pinto la maqueta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiago Elian</t>
   </si>
   <si>
     <t xml:space="preserve">CHIAPPARO</t>
@@ -133,7 +202,37 @@
     <t xml:space="preserve">49419297@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Nazarena Valentina</t>
+    <t xml:space="preserve">Arduino proyecto girasol y sequedad de tierra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">me gusto el segundo modelo, gire e lpanel solar, modeo en tinkercad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venus Yazmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIDANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49735065@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">investigar el codigo con arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grecia De Los Angeles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RODRÍGUEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49626775@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enzo Agustín</t>
   </si>
   <si>
     <t xml:space="preserve">Corbera</t>
@@ -154,31 +253,13 @@
     <t xml:space="preserve">mi ciuidad o parlantito</t>
   </si>
   <si>
-    <t xml:space="preserve">Rafael Bautista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIMÉNEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50156642@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-Pancho pila</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hacer ladron de jouls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kevin Nahuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAIDANA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49735065@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiago Elian</t>
+    <t xml:space="preserve">subir modelos de ciuidades, aspas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idea de la ciudad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramiro Ezequiel</t>
   </si>
   <si>
     <t xml:space="preserve">NUÑEZ</t>
@@ -187,16 +268,10 @@
     <t xml:space="preserve">49589492@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Venus Yazmin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RODRÍGUEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49626775@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grecia De Los Angeles</t>
+    <t xml:space="preserve">motor el circuito andando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benjamin</t>
   </si>
   <si>
     <t xml:space="preserve">ROSALES BASTIDAS</t>
@@ -205,7 +280,10 @@
     <t xml:space="preserve">95429143@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Enzo Agustín</t>
+    <t xml:space="preserve">hacer una ciudad o una pista de aterrizaje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matias</t>
   </si>
   <si>
     <t xml:space="preserve">TASSARA SOTO</t>
@@ -214,33 +292,6 @@
     <t xml:space="preserve">49837749@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Ramiro Ezequiel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TELLO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49676837@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benjamin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEVEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47869497@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trinidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matruia81@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-fuentes</t>
   </si>
   <si>
@@ -277,6 +328,33 @@
     <t xml:space="preserve">Evaluacion</t>
   </si>
   <si>
+    <t xml:space="preserve">explicar generador de continua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maqueta andando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traer el material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">como hacer un estabilizador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">se consiguio modelo para impresora 3d, para la proxima la pila funcionando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hacer 4 pancho pilas para prender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">presentacion con bornes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">separar los bornes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aporte de tevez</t>
+  </si>
+  <si>
     <t xml:space="preserve">le agregaron una bateria</t>
   </si>
   <si>
@@ -289,18 +367,6 @@
     <t xml:space="preserve">acumular extra </t>
   </si>
   <si>
-    <t xml:space="preserve">explicar generador de continua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maqueta andando</t>
-  </si>
-  <si>
-    <t xml:space="preserve">traer el material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">como hacer un estabilizador</t>
-  </si>
-  <si>
     <t xml:space="preserve">automatizado</t>
   </si>
   <si>
@@ -313,12 +379,6 @@
     <t xml:space="preserve">rectificador completo</t>
   </si>
   <si>
-    <t xml:space="preserve">Hacer 4 pancho pilas para prender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">presentacion con bornes</t>
-  </si>
-  <si>
     <t xml:space="preserve">acumulacion</t>
   </si>
   <si>
@@ -328,10 +388,7 @@
     <t xml:space="preserve">imagen vifual?</t>
   </si>
   <si>
-    <t xml:space="preserve">separar los bornes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aporte de tevez</t>
+    <t xml:space="preserve">se compromete para la semana que viene </t>
   </si>
   <si>
     <t xml:space="preserve">Finalizado</t>
@@ -419,9 +476,6 @@
   </si>
   <si>
     <t xml:space="preserve">6 minutos 27 segundos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">4 de abril de 2025  23:17</t>
@@ -508,7 +562,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -525,6 +579,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +596,50 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF232629"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -657,24 +762,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:AF19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T3" activeCellId="0" sqref="T3"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.47"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="31.19"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="13" min="6" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="6" style="0" width="8.61"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="9.71"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="17" min="15" style="0" width="8.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="32.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="36.46"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="15" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="21" min="18" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="22" style="0" width="32.95"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="23" min="23" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="36.46"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="25" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="0" width="56.3"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="65.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,43 +866,67 @@
       <c r="W2" s="2" t="n">
         <v>45907</v>
       </c>
+      <c r="Y2" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="2" t="n">
+        <v>45933</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N3" s="0" t="n">
         <f aca="false">COUNTIF(F3:M3,"P")</f>
@@ -799,123 +934,159 @@
       </c>
       <c r="O3" s="0" t="n">
         <f aca="false">COUNTIF(F3:M3,"C")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U3" s="0" t="n">
-        <f aca="false">ROUND(AVERAGE(T3,R2,P3,N3,L3),0)</f>
-        <v>22956</v>
+        <f aca="false">ROUND(AVERAGE(T3,R3,P3,N3,L3),0)</f>
+        <v>6</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="W3" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC3" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N4" s="0" t="n">
         <f aca="false">COUNTIF(F4:M4,"P")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O4" s="0" t="n">
         <f aca="false">COUNTIF(F4:M4,"C")</f>
         <v>0</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U4" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T4,R4,P4,N4,L4),0)</f>
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF4" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N5" s="0" t="n">
         <f aca="false">COUNTIF(F5:M5,"P")</f>
@@ -923,120 +1094,150 @@
       </c>
       <c r="O5" s="0" t="n">
         <f aca="false">COUNTIF(F5:M5,"C")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U5" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T5,R5,P5,N5,L5),0)</f>
         <v>6</v>
       </c>
-      <c r="V5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="X5" s="0" t="s">
-        <v>26</v>
+      <c r="Y5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N6" s="0" t="n">
         <f aca="false">COUNTIF(F6:M6,"P")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O6" s="0" t="n">
         <f aca="false">COUNTIF(F6:M6,"C")</f>
         <v>0</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U6" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T6,R6,P6,N6,L6),0)</f>
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N7" s="0" t="n">
         <f aca="false">COUNTIF(F7:M7,"P")</f>
@@ -1047,52 +1248,79 @@
         <v>0</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="U7" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T7,R7,P7,N7,L7),0)</f>
         <v>6</v>
       </c>
+      <c r="V7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE7" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N8" s="0" t="n">
         <f aca="false">COUNTIF(F8:M8,"P")</f>
@@ -1103,120 +1331,156 @@
         <v>0</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U8" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T8,R8,P8,N8,L8),0)</f>
         <v>7</v>
       </c>
+      <c r="W8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="N9" s="0" t="n">
         <f aca="false">COUNTIF(F9:M9,"P")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O9" s="0" t="n">
         <f aca="false">COUNTIF(F9:M9,"C")</f>
         <v>0</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="U9" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T9,R9,P9,N9,L9),0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="W9" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="X9" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N10" s="0" t="n">
         <f aca="false">COUNTIF(F10:M10,"P")</f>
@@ -1227,453 +1491,617 @@
         <v>0</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U10" s="0" t="n">
-        <f aca="false">ROUND(AVERAGE(T10,R10,P10,N10,L10),0)</f>
         <v>6</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF10" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N11" s="0" t="n">
         <f aca="false">COUNTIF(F11:M11,"P")</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O11" s="0" t="n">
         <f aca="false">COUNTIF(F11:M11,"C")</f>
         <v>0</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U11" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T11,R11,P11,N11,L11),0)</f>
+        <v>5</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z11" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF11" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N12" s="0" t="n">
         <f aca="false">COUNTIF(F12:M12,"P")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O12" s="0" t="n">
         <f aca="false">COUNTIF(F12:M12,"C")</f>
         <v>0</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U12" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T12,R12,P12,N12,L12),0)</f>
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF12" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N13" s="0" t="n">
         <f aca="false">COUNTIF(F13:M13,"P")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O13" s="0" t="n">
         <f aca="false">COUNTIF(F13:M13,"C")</f>
         <v>0</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="U13" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T13,R13,P13,N13,L13),0)</f>
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC13" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF13" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N14" s="0" t="n">
         <f aca="false">COUNTIF(F14:M14,"P")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O14" s="0" t="n">
         <f aca="false">COUNTIF(F14:M14,"C")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U14" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T14,R14,P14,N14,L14),0)</f>
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF14" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N15" s="0" t="n">
         <f aca="false">COUNTIF(F15:M15,"P")</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O15" s="0" t="n">
         <f aca="false">COUNTIF(F15:M15,"C")</f>
         <v>0</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U15" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T15,R15,P15,N15,L15),0)</f>
+        <v>4</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA15" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF15" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N16" s="0" t="n">
         <f aca="false">COUNTIF(F16:M16,"P")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O16" s="0" t="n">
         <f aca="false">COUNTIF(F16:M16,"C")</f>
         <v>0</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U16" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T16,R16,P16,N16,L16),0)</f>
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="Y16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE16" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>13</v>
+      <c r="I17" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N17" s="0" t="n">
         <f aca="false">COUNTIF(F17:M17,"P")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">COUNTIF(F17:M17,"C")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U17" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T17,R17,P17,N17,L17),0)</f>
-        <v>3</v>
-      </c>
-      <c r="V17" s="0" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="Y17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD17" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF17" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N18" s="0" t="n">
         <f aca="false">COUNTIF(F18:M18,"P")</f>
@@ -1684,14 +2112,29 @@
         <v>0</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U18" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(T18,R18,P18,N18,L18),0)</f>
         <v>7</v>
+      </c>
+      <c r="Y18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF18" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1729,6 +2172,18 @@
       </c>
       <c r="R19" s="0" t="n">
         <f aca="false">COUNTIF(R3:R18,"P")</f>
+        <v>13</v>
+      </c>
+      <c r="Y19" s="0" t="n">
+        <f aca="false">COUNTIF(Y3:Y18,"P")</f>
+        <v>7</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <f aca="false">COUNTIF(AB3:AB18,"P")</f>
+        <v>14</v>
+      </c>
+      <c r="AE19" s="0" t="n">
+        <f aca="false">COUNTIF(AE3:AE18,"P")</f>
         <v>13</v>
       </c>
     </row>
@@ -1748,31 +2203,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:AF19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V18" activeCellId="0" sqref="V18"/>
+      <selection pane="topLeft" activeCell="AF6" activeCellId="0" sqref="AF6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.31"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="4" style="0" width="9.36"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="15.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="10.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="8" style="0" width="9.36"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="11" min="10" style="0" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="10" style="0" width="9.43"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="11.32"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="31.08"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="14" style="0" width="9.43"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="15" style="0" width="19.07"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="16" min="16" style="0" width="9.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="0" width="9.43"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="22.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="32.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="36.46"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="9.5"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="19" style="0" width="22.2"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="21" min="20" style="0" width="9.5"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="22" style="0" width="32.95"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="23" min="23" style="0" width="9.55"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="24" style="0" width="36.46"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="25" style="0" width="9.55"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="0" width="56.3"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="9.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="65.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,37 +2257,37 @@
         <v>4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="O2" s="0" t="s">
         <v>5</v>
@@ -1843,10 +2305,10 @@
         <v>5</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="V2" s="2" t="n">
         <v>45898</v>
@@ -1854,94 +2316,136 @@
       <c r="W2" s="2" t="n">
         <v>45907</v>
       </c>
+      <c r="Y2" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>45919</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>45926</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="2" t="n">
+        <v>45933</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>8</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="0" t="n">
         <f aca="false">G3+H3/2</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D3:F3,I3),0)</f>
-        <v>5</v>
-      </c>
-      <c r="K3" s="3" t="str">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4" t="str">
         <f aca="false">IF(J3&lt;7,"TEP","TEA")</f>
-        <v>TEP</v>
+        <v>TEA</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>7</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="T3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U3" s="5" t="n">
+        <f aca="false">ROUND(AVERAGE(T3,R3,P3,N3,L3),0)</f>
+        <v>7</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC3" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U3" s="3" t="n">
-        <f aca="false">ROUND(AVERAGE(T3,R2,P3,N3,L3),0)</f>
-        <v>9187</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="W3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="X3" s="0" t="s">
-        <v>15</v>
+      <c r="AD3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>8</v>
@@ -1963,73 +2467,88 @@
         <f aca="false">ROUND(AVERAGE(D4:F4,I4),0)</f>
         <v>6</v>
       </c>
-      <c r="K4" s="3" t="str">
+      <c r="K4" s="4" t="str">
         <f aca="false">IF(J4&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="U4" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="U4" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T4,R4,P4,N4,L4),0)</f>
+        <v>7</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF4" s="0" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>8</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="0" t="n">
         <f aca="false">G5+H5/2</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J5" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D5:F5,I5),0)</f>
         <v>8</v>
       </c>
-      <c r="K5" s="3" t="str">
+      <c r="K5" s="4" t="str">
         <f aca="false">IF(J5&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -2037,49 +2556,58 @@
         <v>7</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="O5" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="P5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="U5" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="U5" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T5,R5,P5,N5,L5),0)</f>
-        <v>7</v>
-      </c>
-      <c r="V5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="X5" s="0" t="s">
-        <v>26</v>
+        <v>8</v>
+      </c>
+      <c r="Y5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>7</v>
@@ -2104,16 +2632,13 @@
         <f aca="false">ROUND(AVERAGE(D6:F6,I6),0)</f>
         <v>6</v>
       </c>
-      <c r="K6" s="3" t="str">
+      <c r="K6" s="4" t="str">
         <f aca="false">IF(J6&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="M6" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="N6" s="0" t="n">
         <v>8</v>
       </c>
@@ -2121,260 +2646,335 @@
         <v>6</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="U6" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="U6" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T6,R6,P6,N6,L6),0)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="0" t="n">
         <f aca="false">G7+H7/2</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J7" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D7:F7,I7),0)</f>
-        <v>8</v>
-      </c>
-      <c r="K7" s="3" t="str">
+        <v>3</v>
+      </c>
+      <c r="K7" s="4" t="str">
         <f aca="false">IF(J7&lt;7,"TEP","TEA")</f>
-        <v>TEA</v>
+        <v>TEP</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>7</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>8</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>107</v>
       </c>
       <c r="T7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U7" s="3" t="n">
+      <c r="U7" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T7,R7,P7,N7,L7),0)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="V7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">G8+H8/2</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J8" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D8:F8,I8),0)</f>
-        <v>5</v>
-      </c>
-      <c r="K8" s="3" t="str">
+        <v>2</v>
+      </c>
+      <c r="K8" s="4" t="str">
         <f aca="false">IF(J8&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="U8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="U8" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T8,R8,P8,N8,L8),0)</f>
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">G9+H9/2</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J9" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D9:F9,I9),0)</f>
-        <v>6</v>
-      </c>
-      <c r="K9" s="3" t="str">
+        <v>2</v>
+      </c>
+      <c r="K9" s="4" t="str">
         <f aca="false">IF(J9&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="T9" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="U9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U9" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T9,R9,P9,N9,L9),0)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="W9" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="X9" s="0" t="s">
-        <v>42</v>
+        <v>24</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="0" t="n">
         <f aca="false">G10+H10/2</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J10" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D10:F10,I10),0)</f>
-        <v>3</v>
-      </c>
-      <c r="K10" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="K10" s="4" t="str">
         <f aca="false">IF(J10&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2382,52 +2982,81 @@
         <v>7</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="T10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U10" s="3" t="n">
-        <f aca="false">ROUND(AVERAGE(T10,R10,P10,N10,L10),0)</f>
-        <v>8</v>
+      <c r="U10" s="5" t="n">
+        <v>6</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF10" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G11" s="0" t="n">
         <v>8</v>
@@ -2441,15 +3070,18 @@
       </c>
       <c r="J11" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D11:F11,I11),0)</f>
-        <v>8</v>
-      </c>
-      <c r="K11" s="3" t="str">
+        <v>6</v>
+      </c>
+      <c r="K11" s="4" t="str">
         <f aca="false">IF(J11&lt;7,"TEP","TEA")</f>
-        <v>TEA</v>
+        <v>TEP</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="M11" s="0" t="s">
+        <v>112</v>
+      </c>
       <c r="N11" s="0" t="n">
         <v>7</v>
       </c>
@@ -2457,31 +3089,52 @@
         <v>8</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>113</v>
       </c>
       <c r="T11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="U11" s="5" t="n">
+        <f aca="false">ROUND(AVERAGE(T11,R11,P11,N11,L11),0)</f>
+        <v>8</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC11" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U11" s="3" t="n">
-        <f aca="false">ROUND(AVERAGE(T11,R11,P11,N11,L11),0)</f>
-        <v>8</v>
+      <c r="AD11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF11" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>8</v>
@@ -2501,62 +3154,80 @@
       </c>
       <c r="J12" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D12:F12,I12),0)</f>
-        <v>6</v>
-      </c>
-      <c r="K12" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="K12" s="4" t="str">
         <f aca="false">IF(J12&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="O12" s="0" t="s">
-        <v>99</v>
-      </c>
       <c r="P12" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="T12" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="U12" s="3" t="n">
+      <c r="U12" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T12,R12,P12,N12,L12),0)</f>
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF12" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>8</v>
@@ -2570,11 +3241,11 @@
       </c>
       <c r="J13" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D13:F13,I13),0)</f>
-        <v>5</v>
-      </c>
-      <c r="K13" s="3" t="str">
+        <v>8</v>
+      </c>
+      <c r="K13" s="4" t="str">
         <f aca="false">IF(J13&lt;7,"TEP","TEA")</f>
-        <v>TEP</v>
+        <v>TEA</v>
       </c>
       <c r="L13" s="0" t="n">
         <v>8</v>
@@ -2586,37 +3257,58 @@
         <v>8</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="T13" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="U13" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="U13" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T13,R13,P13,N13,L13),0)</f>
+        <v>8</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC13" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF13" s="0" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>8</v>
@@ -2630,50 +3322,59 @@
       </c>
       <c r="J14" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D14:F14,I14),0)</f>
-        <v>7</v>
-      </c>
-      <c r="K14" s="3" t="str">
+        <v>5</v>
+      </c>
+      <c r="K14" s="4" t="str">
         <f aca="false">IF(J14&lt;7,"TEP","TEA")</f>
-        <v>TEA</v>
+        <v>TEP</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>7</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="U14" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="U14" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T14,R14,P14,N14,L14),0)</f>
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF14" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>8</v>
@@ -2685,206 +3386,287 @@
         <v>8</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15" s="0" t="n">
         <f aca="false">G15+H15/2</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J15" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D15:F15,I15),0)</f>
         <v>6</v>
       </c>
-      <c r="K15" s="3" t="str">
+      <c r="K15" s="4" t="str">
         <f aca="false">IF(J15&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
       <c r="L15" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="M15" s="0" t="s">
+        <v>116</v>
+      </c>
       <c r="N15" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="O15" s="0" t="s">
+        <v>117</v>
+      </c>
       <c r="P15" s="0" t="n">
         <v>6</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>117</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="U15" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="U15" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T15,R15,P15,N15,L15),0)</f>
+        <v>7</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC15" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF15" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">G16+H16/2</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J16" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D16:F16,I16),0)</f>
-        <v>2</v>
-      </c>
-      <c r="K16" s="3" t="str">
+        <v>6</v>
+      </c>
+      <c r="K16" s="4" t="str">
         <f aca="false">IF(J16&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="M16" s="0" t="s">
+        <v>118</v>
+      </c>
       <c r="N16" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>119</v>
       </c>
       <c r="P16" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="U16" s="5" t="n">
+        <f aca="false">ROUND(AVERAGE(T16,R16,P16,N16,L16),0)</f>
+        <v>7</v>
+      </c>
+      <c r="Y16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA16" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC16" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF16" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="R16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="S16" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="T16" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="U16" s="3" t="n">
-        <f aca="false">ROUND(AVERAGE(T16,R16,P16,N16,L16),0)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="I17" s="0" t="n">
         <f aca="false">G17+H17/2</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J17" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D17:F17,I17),0)</f>
+        <v>7</v>
+      </c>
+      <c r="K17" s="4" t="str">
+        <f aca="false">IF(J17&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="R17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="U17" s="5" t="n">
+        <f aca="false">ROUND(AVERAGE(T17,R17,P17,N17,L17),0)</f>
+        <v>7</v>
+      </c>
+      <c r="Y17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD17" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF17" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H18" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="K17" s="3" t="str">
-        <f aca="false">IF(J17&lt;7,"TEP","TEA")</f>
-        <v>TEP</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="P17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="R17" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="S17" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="T17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U17" s="3" t="n">
-        <f aca="false">ROUND(AVERAGE(T17,R17,P17,N17,L17),0)</f>
-        <v>4</v>
-      </c>
-      <c r="V17" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="I18" s="0" t="n">
         <f aca="false">G18+H18/2</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J18" s="3" t="n">
         <f aca="false">ROUND(AVERAGE(D18:F18,I18),0)</f>
         <v>6</v>
       </c>
-      <c r="K18" s="3" t="str">
+      <c r="K18" s="4" t="str">
         <f aca="false">IF(J18&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -2892,22 +3674,46 @@
         <v>7</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P18" s="0" t="n">
         <v>6</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T18" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="U18" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="U18" s="5" t="n">
         <f aca="false">ROUND(AVERAGE(T18,R18,P18,N18,L18),0)</f>
+        <v>7</v>
+      </c>
+      <c r="Y18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z18" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA18" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD18" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF18" s="0" t="n">
         <v>8</v>
       </c>
     </row>
@@ -2920,27 +3726,39 @@
         <f aca="false">COUNTIF(R3:R18,"P")</f>
         <v>13</v>
       </c>
+      <c r="Y19" s="0" t="n">
+        <f aca="false">COUNTIF(Y3:Y18,"P")</f>
+        <v>7</v>
+      </c>
+      <c r="AB19" s="0" t="n">
+        <f aca="false">COUNTIF(AB3:AB18,"P")</f>
+        <v>14</v>
+      </c>
+      <c r="AE19" s="0" t="n">
+        <f aca="false">COUNTIF(AE3:AE18,"P")</f>
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J3:J18">
-    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K18">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>"TEP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U3:U18">
-    <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="notBetween" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="5" operator="notBetween" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>4</formula>
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="6" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2965,7 +3783,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.95"/>
@@ -2977,22 +3795,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3000,7 +3818,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1</v>
@@ -3014,16 +3832,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>8</v>
@@ -3037,16 +3855,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>5</v>
@@ -3060,16 +3878,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>7</v>
@@ -3083,16 +3901,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>7</v>
@@ -3106,16 +3924,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>3</v>
@@ -3129,16 +3947,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>9</v>
@@ -3157,13 +3975,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>1</v>
@@ -3174,16 +3992,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>2</v>
@@ -3197,16 +4015,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>7</v>
@@ -3220,16 +4038,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>7</v>
@@ -3248,13 +4066,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>5</v>
@@ -3265,16 +4083,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>1</v>
@@ -3288,16 +4106,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>2</v>
@@ -3311,16 +4129,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>6</v>
@@ -3334,16 +4152,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>132</v>
+        <v>68</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1</v>
@@ -3357,7 +4175,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>1</v>
@@ -3371,16 +4189,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>7</v>
@@ -3411,7 +4229,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.57"/>
   </cols>
@@ -3430,10 +4248,10 @@
         <v>45751</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3441,7 +4259,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">C2+D2</f>
@@ -3456,7 +4274,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">C3+D3</f>
@@ -3471,7 +4289,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2</v>
@@ -3486,7 +4304,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">C5+D5</f>
@@ -3498,7 +4316,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">C6+D6</f>
@@ -3510,7 +4328,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">C7+D7</f>
@@ -3525,7 +4343,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">C8+D8</f>
@@ -3537,7 +4355,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">C9+D9</f>
@@ -3552,7 +4370,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">C10+D10</f>
@@ -3567,7 +4385,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">C11+D11</f>
@@ -3579,7 +4397,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">C12+D12</f>
@@ -3591,7 +4409,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">C13+D13</f>
@@ -3603,7 +4421,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1</v>
@@ -3621,7 +4439,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">C15+D15</f>
@@ -3633,7 +4451,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">C16+D16</f>
@@ -3645,7 +4463,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">C17+D17</f>

</xml_diff>